<commit_message>
Add market value calculation
</commit_message>
<xml_diff>
--- a/etf_top_holdings.xlsx
+++ b/etf_top_holdings.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,11 @@
           <t>Holding Percent</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>holding_value</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -474,6 +479,9 @@
       <c r="D2" t="n">
         <v>0.088809796</v>
       </c>
+      <c r="E2" t="n">
+        <v>365.02</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -494,6 +502,9 @@
       <c r="D3" t="n">
         <v>0.0733159</v>
       </c>
+      <c r="E3" t="n">
+        <v>301.33</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -514,6 +525,9 @@
       <c r="D4" t="n">
         <v>0.061153304</v>
       </c>
+      <c r="E4" t="n">
+        <v>251.34</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -534,6 +548,9 @@
       <c r="D5" t="n">
         <v>0.0489161</v>
       </c>
+      <c r="E5" t="n">
+        <v>201.05</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -554,6 +571,9 @@
       <c r="D6" t="n">
         <v>0.040236503</v>
       </c>
+      <c r="E6" t="n">
+        <v>165.38</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -574,6 +594,9 @@
       <c r="D7" t="n">
         <v>0.037602</v>
       </c>
+      <c r="E7" t="n">
+        <v>154.55</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -594,6 +617,9 @@
       <c r="D8" t="n">
         <v>0.0364074</v>
       </c>
+      <c r="E8" t="n">
+        <v>149.64</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -614,6 +640,9 @@
       <c r="D9" t="n">
         <v>0.0350006</v>
       </c>
+      <c r="E9" t="n">
+        <v>143.86</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -634,6 +663,9 @@
       <c r="D10" t="n">
         <v>0.0307373</v>
       </c>
+      <c r="E10" t="n">
+        <v>126.33</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -654,6 +686,9 @@
       <c r="D11" t="n">
         <v>0.029916698</v>
       </c>
+      <c r="E11" t="n">
+        <v>122.96</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -674,6 +709,9 @@
       <c r="D12" t="n">
         <v>0.0491187</v>
       </c>
+      <c r="E12" t="n">
+        <v>444.17</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -694,6 +732,9 @@
       <c r="D13" t="n">
         <v>0.043710798</v>
       </c>
+      <c r="E13" t="n">
+        <v>395.26</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -714,6 +755,9 @@
       <c r="D14" t="n">
         <v>0.043211497</v>
       </c>
+      <c r="E14" t="n">
+        <v>390.75</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -734,6 +778,9 @@
       <c r="D15" t="n">
         <v>0.0420383</v>
       </c>
+      <c r="E15" t="n">
+        <v>380.14</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -754,6 +801,9 @@
       <c r="D16" t="n">
         <v>0.0405344</v>
       </c>
+      <c r="E16" t="n">
+        <v>366.54</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -774,6 +824,9 @@
       <c r="D17" t="n">
         <v>0.040001</v>
       </c>
+      <c r="E17" t="n">
+        <v>361.72</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -794,6 +847,9 @@
       <c r="D18" t="n">
         <v>0.0399257</v>
       </c>
+      <c r="E18" t="n">
+        <v>361.04</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -814,6 +870,9 @@
       <c r="D19" t="n">
         <v>0.0392987</v>
       </c>
+      <c r="E19" t="n">
+        <v>355.37</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -834,6 +893,9 @@
       <c r="D20" t="n">
         <v>0.0391208</v>
       </c>
+      <c r="E20" t="n">
+        <v>353.76</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -854,6 +916,9 @@
       <c r="D21" t="n">
         <v>0.0387548</v>
       </c>
+      <c r="E21" t="n">
+        <v>350.45</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -874,6 +939,9 @@
       <c r="D22" t="n">
         <v>0.1143839</v>
       </c>
+      <c r="E22" t="n">
+        <v>410.14</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -894,6 +962,9 @@
       <c r="D23" t="n">
         <v>0.09441869999999999</v>
       </c>
+      <c r="E23" t="n">
+        <v>338.55</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -914,6 +985,9 @@
       <c r="D24" t="n">
         <v>0.078748494</v>
       </c>
+      <c r="E24" t="n">
+        <v>282.36</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -934,6 +1008,9 @@
       <c r="D25" t="n">
         <v>0.0573034</v>
       </c>
+      <c r="E25" t="n">
+        <v>205.47</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -954,6 +1031,9 @@
       <c r="D26" t="n">
         <v>0.0496094</v>
       </c>
+      <c r="E26" t="n">
+        <v>177.88</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -974,6 +1054,9 @@
       <c r="D27" t="n">
         <v>0.0484242</v>
       </c>
+      <c r="E27" t="n">
+        <v>173.63</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -994,6 +1077,9 @@
       <c r="D28" t="n">
         <v>0.0426679</v>
       </c>
+      <c r="E28" t="n">
+        <v>152.99</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1014,6 +1100,9 @@
       <c r="D29" t="n">
         <v>0.0387571</v>
       </c>
+      <c r="E29" t="n">
+        <v>138.97</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1034,6 +1123,9 @@
       <c r="D30" t="n">
         <v>0.0385587</v>
       </c>
+      <c r="E30" t="n">
+        <v>138.26</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1054,6 +1146,9 @@
       <c r="D31" t="n">
         <v>0.0295715</v>
       </c>
+      <c r="E31" t="n">
+        <v>106.03</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1074,6 +1169,9 @@
       <c r="D32" t="n">
         <v>0.14764869</v>
       </c>
+      <c r="E32" t="n">
+        <v>1353.17</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1094,6 +1192,9 @@
       <c r="D33" t="n">
         <v>0.101668194</v>
       </c>
+      <c r="E33" t="n">
+        <v>931.77</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1114,6 +1215,9 @@
       <c r="D34" t="n">
         <v>0.0625163</v>
       </c>
+      <c r="E34" t="n">
+        <v>572.95</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1134,6 +1238,9 @@
       <c r="D35" t="n">
         <v>0.0609458</v>
       </c>
+      <c r="E35" t="n">
+        <v>558.55</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1154,6 +1261,9 @@
       <c r="D36" t="n">
         <v>0.050044797</v>
       </c>
+      <c r="E36" t="n">
+        <v>458.65</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1174,6 +1284,9 @@
       <c r="D37" t="n">
         <v>0.049737703</v>
       </c>
+      <c r="E37" t="n">
+        <v>455.83</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1194,6 +1307,9 @@
       <c r="D38" t="n">
         <v>0.049608696</v>
       </c>
+      <c r="E38" t="n">
+        <v>454.65</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1214,6 +1330,9 @@
       <c r="D39" t="n">
         <v>0.0392244</v>
       </c>
+      <c r="E39" t="n">
+        <v>359.48</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1234,6 +1353,9 @@
       <c r="D40" t="n">
         <v>0.0280142</v>
       </c>
+      <c r="E40" t="n">
+        <v>256.74</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1254,6 +1376,9 @@
       <c r="D41" t="n">
         <v>0.026184399</v>
       </c>
+      <c r="E41" t="n">
+        <v>239.97</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1274,6 +1399,9 @@
       <c r="D42" t="n">
         <v>0.180532</v>
       </c>
+      <c r="E42" t="n">
+        <v>583.08</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1294,6 +1422,9 @@
       <c r="D43" t="n">
         <v>0.14334561</v>
       </c>
+      <c r="E43" t="n">
+        <v>462.98</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1314,6 +1445,9 @@
       <c r="D44" t="n">
         <v>0.109383</v>
       </c>
+      <c r="E44" t="n">
+        <v>353.28</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1334,6 +1468,9 @@
       <c r="D45" t="n">
         <v>0.0432814</v>
       </c>
+      <c r="E45" t="n">
+        <v>139.79</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1354,6 +1491,9 @@
       <c r="D46" t="n">
         <v>0.0235007</v>
       </c>
+      <c r="E46" t="n">
+        <v>75.90000000000001</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1374,6 +1514,9 @@
       <c r="D47" t="n">
         <v>0.0189585</v>
       </c>
+      <c r="E47" t="n">
+        <v>61.23</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1394,6 +1537,9 @@
       <c r="D48" t="n">
         <v>0.0162414</v>
       </c>
+      <c r="E48" t="n">
+        <v>52.46</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1414,6 +1560,9 @@
       <c r="D49" t="n">
         <v>0.0155648</v>
       </c>
+      <c r="E49" t="n">
+        <v>50.27</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1434,6 +1583,9 @@
       <c r="D50" t="n">
         <v>0.0151909</v>
       </c>
+      <c r="E50" t="n">
+        <v>49.06</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1454,6 +1606,9 @@
       <c r="D51" t="n">
         <v>0.014360799</v>
       </c>
+      <c r="E51" t="n">
+        <v>46.38</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1474,6 +1629,9 @@
       <c r="D52" t="n">
         <v>0.07827580000000001</v>
       </c>
+      <c r="E52" t="n">
+        <v>1863.97</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1494,6 +1652,9 @@
       <c r="D53" t="n">
         <v>0.06461989999999999</v>
       </c>
+      <c r="E53" t="n">
+        <v>1538.78</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1514,6 +1675,9 @@
       <c r="D54" t="n">
         <v>0.053899</v>
       </c>
+      <c r="E54" t="n">
+        <v>1283.49</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1534,6 +1698,9 @@
       <c r="D55" t="n">
         <v>0.0392343</v>
       </c>
+      <c r="E55" t="n">
+        <v>934.28</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1554,6 +1721,9 @@
       <c r="D56" t="n">
         <v>0.033143</v>
       </c>
+      <c r="E56" t="n">
+        <v>789.23</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1574,6 +1744,9 @@
       <c r="D57" t="n">
         <v>0.026530199</v>
       </c>
+      <c r="E57" t="n">
+        <v>631.76</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1594,6 +1767,9 @@
       <c r="D58" t="n">
         <v>0.0263679</v>
       </c>
+      <c r="E58" t="n">
+        <v>627.89</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1614,6 +1790,9 @@
       <c r="D59" t="n">
         <v>0.0262994</v>
       </c>
+      <c r="E59" t="n">
+        <v>626.26</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1634,6 +1813,9 @@
       <c r="D60" t="n">
         <v>0.020383101</v>
       </c>
+      <c r="E60" t="n">
+        <v>485.38</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1654,6 +1836,9 @@
       <c r="D61" t="n">
         <v>0.0148507</v>
       </c>
+      <c r="E61" t="n">
+        <v>353.64</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1674,6 +1859,9 @@
       <c r="D62" t="n">
         <v>0.0661532</v>
       </c>
+      <c r="E62" t="n">
+        <v>910.49</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1694,6 +1882,9 @@
       <c r="D63" t="n">
         <v>0.057487402</v>
       </c>
+      <c r="E63" t="n">
+        <v>791.22</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1714,6 +1905,9 @@
       <c r="D64" t="n">
         <v>0.0479509</v>
       </c>
+      <c r="E64" t="n">
+        <v>659.97</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1734,6 +1928,9 @@
       <c r="D65" t="n">
         <v>0.034518298</v>
       </c>
+      <c r="E65" t="n">
+        <v>475.09</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1754,6 +1951,9 @@
       <c r="D66" t="n">
         <v>0.0294768</v>
       </c>
+      <c r="E66" t="n">
+        <v>405.7</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1774,6 +1974,9 @@
       <c r="D67" t="n">
         <v>0.0234558</v>
       </c>
+      <c r="E67" t="n">
+        <v>322.83</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1794,6 +1997,9 @@
       <c r="D68" t="n">
         <v>0.023395099</v>
       </c>
+      <c r="E68" t="n">
+        <v>322</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1814,6 +2020,9 @@
       <c r="D69" t="n">
         <v>0.023333099</v>
       </c>
+      <c r="E69" t="n">
+        <v>321.14</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1834,6 +2043,9 @@
       <c r="D70" t="n">
         <v>0.0182412</v>
       </c>
+      <c r="E70" t="n">
+        <v>251.06</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1853,6 +2065,9 @@
       </c>
       <c r="D71" t="n">
         <v>0.0132287005</v>
+      </c>
+      <c r="E71" t="n">
+        <v>182.07</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add sector for each ticker
</commit_message>
<xml_diff>
--- a/etf_top_holdings.xlsx
+++ b/etf_top_holdings.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,11 @@
           <t>holding_value</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Sector</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -482,6 +487,11 @@
       <c r="E2" t="n">
         <v>365.02</v>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -505,6 +515,11 @@
       <c r="E3" t="n">
         <v>301.33</v>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -528,6 +543,11 @@
       <c r="E4" t="n">
         <v>251.34</v>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -551,6 +571,11 @@
       <c r="E5" t="n">
         <v>201.05</v>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Consumer Cyclical</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -574,6 +599,11 @@
       <c r="E6" t="n">
         <v>165.38</v>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Communication Services</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -597,6 +627,11 @@
       <c r="E7" t="n">
         <v>154.55</v>
       </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Communication Services</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -620,6 +655,11 @@
       <c r="E8" t="n">
         <v>149.64</v>
       </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Consumer Cyclical</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -643,6 +683,11 @@
       <c r="E9" t="n">
         <v>143.86</v>
       </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Communication Services</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -666,6 +711,11 @@
       <c r="E10" t="n">
         <v>126.33</v>
       </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Consumer Defensive</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -689,6 +739,11 @@
       <c r="E11" t="n">
         <v>122.96</v>
       </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -712,6 +767,11 @@
       <c r="E12" t="n">
         <v>444.17</v>
       </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Industrials</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -735,6 +795,11 @@
       <c r="E13" t="n">
         <v>395.26</v>
       </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -758,6 +823,11 @@
       <c r="E14" t="n">
         <v>390.75</v>
       </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Energy</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -781,6 +851,11 @@
       <c r="E15" t="n">
         <v>380.14</v>
       </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Energy</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -804,6 +879,11 @@
       <c r="E16" t="n">
         <v>366.54</v>
       </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Communication Services</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -827,6 +907,11 @@
       <c r="E17" t="n">
         <v>361.72</v>
       </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Healthcare</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -850,6 +935,11 @@
       <c r="E18" t="n">
         <v>361.04</v>
       </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Healthcare</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -873,6 +963,11 @@
       <c r="E19" t="n">
         <v>355.37</v>
       </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Consumer Defensive</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -896,6 +991,11 @@
       <c r="E20" t="n">
         <v>353.76</v>
       </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Consumer Defensive</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -919,6 +1019,11 @@
       <c r="E21" t="n">
         <v>350.45</v>
       </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Consumer Cyclical</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -942,6 +1047,11 @@
       <c r="E22" t="n">
         <v>410.14</v>
       </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -965,6 +1075,11 @@
       <c r="E23" t="n">
         <v>338.55</v>
       </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -988,6 +1103,11 @@
       <c r="E24" t="n">
         <v>282.36</v>
       </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1011,6 +1131,11 @@
       <c r="E25" t="n">
         <v>205.47</v>
       </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Consumer Cyclical</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1034,6 +1159,11 @@
       <c r="E26" t="n">
         <v>177.88</v>
       </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Communication Services</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1057,6 +1187,11 @@
       <c r="E27" t="n">
         <v>173.63</v>
       </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Communication Services</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1080,6 +1215,11 @@
       <c r="E28" t="n">
         <v>152.99</v>
       </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Consumer Cyclical</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1103,6 +1243,11 @@
       <c r="E29" t="n">
         <v>138.97</v>
       </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Communication Services</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1126,6 +1271,11 @@
       <c r="E30" t="n">
         <v>138.26</v>
       </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1149,6 +1299,11 @@
       <c r="E31" t="n">
         <v>106.03</v>
       </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Healthcare</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1172,6 +1327,11 @@
       <c r="E32" t="n">
         <v>1353.17</v>
       </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1195,6 +1355,11 @@
       <c r="E33" t="n">
         <v>931.77</v>
       </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1218,6 +1383,11 @@
       <c r="E34" t="n">
         <v>572.95</v>
       </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Communication Services</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1241,6 +1411,11 @@
       <c r="E35" t="n">
         <v>558.55</v>
       </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1264,6 +1439,11 @@
       <c r="E36" t="n">
         <v>458.65</v>
       </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Communication Services</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1287,6 +1467,11 @@
       <c r="E37" t="n">
         <v>455.83</v>
       </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1310,6 +1495,11 @@
       <c r="E38" t="n">
         <v>454.65</v>
       </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Communication Services</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1333,6 +1523,11 @@
       <c r="E39" t="n">
         <v>359.48</v>
       </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Consumer Cyclical</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1356,6 +1551,11 @@
       <c r="E40" t="n">
         <v>256.74</v>
       </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Financial Services</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1379,6 +1579,11 @@
       <c r="E41" t="n">
         <v>239.97</v>
       </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Healthcare</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1402,6 +1607,11 @@
       <c r="E42" t="n">
         <v>583.08</v>
       </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1425,6 +1635,11 @@
       <c r="E43" t="n">
         <v>462.98</v>
       </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1448,6 +1663,11 @@
       <c r="E44" t="n">
         <v>353.28</v>
       </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1471,6 +1691,11 @@
       <c r="E45" t="n">
         <v>139.79</v>
       </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1494,6 +1719,11 @@
       <c r="E46" t="n">
         <v>75.90000000000001</v>
       </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1517,6 +1747,11 @@
       <c r="E47" t="n">
         <v>61.23</v>
       </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1540,6 +1775,11 @@
       <c r="E48" t="n">
         <v>52.46</v>
       </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1563,6 +1803,11 @@
       <c r="E49" t="n">
         <v>50.27</v>
       </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1586,6 +1831,11 @@
       <c r="E50" t="n">
         <v>49.06</v>
       </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1609,6 +1859,11 @@
       <c r="E51" t="n">
         <v>46.38</v>
       </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1632,6 +1887,11 @@
       <c r="E52" t="n">
         <v>1863.97</v>
       </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1655,6 +1915,11 @@
       <c r="E53" t="n">
         <v>1538.78</v>
       </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1678,6 +1943,11 @@
       <c r="E54" t="n">
         <v>1283.49</v>
       </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1701,6 +1971,11 @@
       <c r="E55" t="n">
         <v>934.28</v>
       </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Consumer Cyclical</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1724,6 +1999,11 @@
       <c r="E56" t="n">
         <v>789.23</v>
       </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Communication Services</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1747,6 +2027,11 @@
       <c r="E57" t="n">
         <v>631.76</v>
       </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Communication Services</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1770,6 +2055,11 @@
       <c r="E58" t="n">
         <v>627.89</v>
       </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1793,6 +2083,11 @@
       <c r="E59" t="n">
         <v>626.26</v>
       </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Communication Services</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1816,6 +2111,11 @@
       <c r="E60" t="n">
         <v>485.38</v>
       </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Consumer Cyclical</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1839,6 +2139,11 @@
       <c r="E61" t="n">
         <v>353.64</v>
       </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Financial Services</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1862,6 +2167,11 @@
       <c r="E62" t="n">
         <v>910.49</v>
       </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1885,6 +2195,11 @@
       <c r="E63" t="n">
         <v>791.22</v>
       </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1908,6 +2223,11 @@
       <c r="E64" t="n">
         <v>659.97</v>
       </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1931,6 +2251,11 @@
       <c r="E65" t="n">
         <v>475.09</v>
       </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Consumer Cyclical</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1954,6 +2279,11 @@
       <c r="E66" t="n">
         <v>405.7</v>
       </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Communication Services</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1977,6 +2307,11 @@
       <c r="E67" t="n">
         <v>322.83</v>
       </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Technology</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2000,6 +2335,11 @@
       <c r="E68" t="n">
         <v>322</v>
       </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Communication Services</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2023,6 +2363,11 @@
       <c r="E69" t="n">
         <v>321.14</v>
       </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Communication Services</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2046,6 +2391,11 @@
       <c r="E70" t="n">
         <v>251.06</v>
       </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Consumer Cyclical</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2068,6 +2418,11 @@
       </c>
       <c r="E71" t="n">
         <v>182.07</v>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Healthcare</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>